<commit_message>
Various changes, added comments
</commit_message>
<xml_diff>
--- a/docs/example_2_wadied.xlsx
+++ b/docs/example_2_wadied.xlsx
@@ -570,42 +570,42 @@
       <c r="D2" s="1" t="inlineStr"/>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mg / (1l)</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mg / (1l)</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mmol / (1l)</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mg / (1l)</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mg / (1l)</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mg / (1l)</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mg / (1l)</t>
         </is>
       </c>
       <c r="L2" s="1" t="inlineStr">
         <is>
-          <t>mmol / l</t>
+          <t>mg / (1l)</t>
         </is>
       </c>
       <c r="M2" s="1" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>µmol / l</t>
+          <t>ug / (1l)</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr"/>
@@ -671,23 +671,23 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>&lt;0.01052948771474189</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H4" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>&lt;0.024951344877488894</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -706,7 +706,7 @@
         <v>100</v>
       </c>
       <c r="O4" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P4" t="n">
         <v>1</v>
@@ -746,23 +746,23 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>&lt;0.01052948771474189</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H5" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>-0.02495134487748889</v>
+        <v>-1</v>
       </c>
       <c r="M5" t="n">
         <v>1</v>
@@ -779,7 +779,7 @@
         <v>100</v>
       </c>
       <c r="O5" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P5" t="n">
         <v>1</v>
@@ -811,23 +811,23 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>&lt;0.01052948771474189</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H6" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
@@ -842,7 +842,7 @@
         <v>100</v>
       </c>
       <c r="O6" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P6" t="n">
         <v>1</v>
@@ -874,27 +874,27 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>&lt;0.01052948771474189</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H7" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
-        <v>0.02495134487748889</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
         <v>1</v>
@@ -903,7 +903,7 @@
         <v>100</v>
       </c>
       <c r="O7" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P7" t="n">
         <v>1</v>
@@ -936,26 +936,26 @@
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.01052948771474189</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H8" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="n">
-        <v>0.02495134487748889</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
         <v>1</v>
@@ -964,7 +964,7 @@
         <v>100</v>
       </c>
       <c r="O8" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P8" t="n">
         <v>1</v>
@@ -995,27 +995,27 @@
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>0.01052948771474189</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H9" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>&lt;0.024951344877488894</t>
+          <t>&lt;1</t>
         </is>
       </c>
       <c r="M9" t="n">
@@ -1025,7 +1025,7 @@
         <v>100</v>
       </c>
       <c r="O9" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P9" t="n">
         <v>1</v>
@@ -1056,26 +1056,26 @@
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>0.01052948771474189</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H10" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
-        <v>-0.02495134487748889</v>
+        <v>-1</v>
       </c>
       <c r="M10" t="n">
         <v>1</v>
@@ -1084,7 +1084,7 @@
         <v>100</v>
       </c>
       <c r="O10" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P10" t="n">
         <v>1</v>
@@ -1117,22 +1117,22 @@
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>0.01052948771474189</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.01612775296307948</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
         <v>0.02173653150166828</v>
       </c>
       <c r="H11" t="n">
-        <v>0.05543708342843102</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01664328008426826</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>0.01040989806419618</v>
+        <v>1</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
@@ -1147,7 +1147,7 @@
         <v>100</v>
       </c>
       <c r="O11" t="n">
-        <v>13.3472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P11" t="n">
         <v>1</v>
@@ -1178,26 +1178,26 @@
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.01052948993260274</v>
+        <v>0.3261379151327745</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01612775419066612</v>
+        <v>225.8966630056657</v>
       </c>
       <c r="G12" t="n">
-        <v>0.02173653150166828</v>
+        <v>21.73653150166828</v>
       </c>
       <c r="H12" t="n">
-        <v>0.05543709306763623</v>
+        <v>0.7764908977817396</v>
       </c>
       <c r="I12" t="n">
-        <v>0.01664328285425644</v>
+        <v>0.4674349206032192</v>
       </c>
       <c r="J12" t="n">
-        <v>0.01040994348861396</v>
+        <v>0.3337927559737088</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
-        <v>0.02495134487748889</v>
+        <v>1000</v>
       </c>
       <c r="M12" t="n">
         <v>1</v>
@@ -1206,7 +1206,7 @@
         <v>100</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0133472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P12" t="n">
         <v>1</v>
@@ -1237,26 +1237,26 @@
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>0.01052948993260274</v>
+        <v>0.3261379151327745</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01612775419066612</v>
+        <v>225.8966630056657</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02173653150166828</v>
+        <v>21.73653150166828</v>
       </c>
       <c r="H13" t="n">
-        <v>0.05543709306763623</v>
+        <v>0.7764908977817396</v>
       </c>
       <c r="I13" t="n">
-        <v>0.01664328285425644</v>
+        <v>0.4674349206032192</v>
       </c>
       <c r="J13" t="n">
-        <v>0.01040994348861396</v>
+        <v>0.3337927559737088</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
-        <v>0.02495134487748889</v>
+        <v>1000</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
@@ -1265,7 +1265,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0133472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P13" t="n">
         <v>1</v>
@@ -1299,27 +1299,27 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>&lt;0.010529489766889116</t>
+          <t>&lt;0.32613791</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.01612775419066612</v>
+        <v>225.8966630056657</v>
       </c>
       <c r="G14" t="n">
-        <v>0.02173653150166828</v>
+        <v>21.73653150166828</v>
       </c>
       <c r="H14" t="n">
-        <v>0.05543709306763623</v>
+        <v>0.7764908977817396</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01664328285425644</v>
+        <v>0.4674349206032192</v>
       </c>
       <c r="J14" t="n">
-        <v>0.01040994348861396</v>
+        <v>0.3337927559737088</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
-        <v>0.02495134487748889</v>
+        <v>1000</v>
       </c>
       <c r="M14" t="n">
         <v>1</v>
@@ -1328,7 +1328,7 @@
         <v>100</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0133472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P14" t="n">
         <v>1</v>
@@ -1360,27 +1360,27 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>&lt;0.010529489766889116</t>
+          <t>&lt;0.32613791</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.01612775419066612</v>
+        <v>225.8966630056657</v>
       </c>
       <c r="G15" t="n">
-        <v>0.02173653150166828</v>
+        <v>21.73653150166828</v>
       </c>
       <c r="H15" t="n">
-        <v>0.05543709306763623</v>
+        <v>0.7764908977817396</v>
       </c>
       <c r="I15" t="n">
-        <v>0.01664328285425644</v>
+        <v>0.4674349206032192</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01040994348861396</v>
+        <v>0.3337927559737088</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="n">
-        <v>0.02495134487748889</v>
+        <v>1000</v>
       </c>
       <c r="M15" t="n">
         <v>1</v>
@@ -1389,7 +1389,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0133472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P15" t="n">
         <v>1</v>
@@ -1421,27 +1421,27 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>&lt;0.010529489766889116</t>
+          <t>&lt;0.32613791</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.01612775419066612</v>
+        <v>225.8966630056657</v>
       </c>
       <c r="G16" t="n">
-        <v>0.02173653150166828</v>
+        <v>21.73653150166828</v>
       </c>
       <c r="H16" t="n">
-        <v>0.05543709306763623</v>
+        <v>0.7764908977817396</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01664328285425644</v>
+        <v>0.4674349206032192</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01040994348861396</v>
+        <v>0.3337927559737088</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
-        <v>0.02495134487748889</v>
+        <v>1000</v>
       </c>
       <c r="M16" t="n">
         <v>1</v>
@@ -1450,7 +1450,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0133472865867311</v>
+        <v>1000</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>

</xml_diff>